<commit_message>
player_logs folder is created
</commit_message>
<xml_diff>
--- a/backend/jupyter/action_volume/data/player_action_hyper.xlsx
+++ b/backend/jupyter/action_volume/data/player_action_hyper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\okany\Documents\GitHub\football-simulation-game\backend\jupyter\action_volume\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6F7AE3-653F-4ED1-9B34-65B70FD7477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AECAD21-12DE-4338-BB44-0213BFE19EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2715" yWindow="1710" windowWidth="23445" windowHeight="12960" xr2:uid="{80BC0565-8455-4789-85AC-BADDCAB4FB5F}"/>
   </bookViews>
@@ -539,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF87F7AE-31A1-4258-A843-2616A13931FE}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>

</xml_diff>